<commit_message>
Corecting results - using other paramters get better results
</commit_message>
<xml_diff>
--- a/comparatie-clasificatori/comparatie-evalure-all-cclassifieries.xlsx
+++ b/comparatie-clasificatori/comparatie-evalure-all-cclassifieries.xlsx
@@ -455,13 +455,13 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>95.64</v>
+        <v>96.69</v>
       </c>
       <c r="C4">
-        <v>95.7</v>
+        <v>96.6</v>
       </c>
       <c r="D4">
-        <v>95.6</v>
+        <v>96.7</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -479,7 +479,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -525,13 +525,13 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>96.435500000000005</v>
+        <v>97.46</v>
       </c>
       <c r="C4">
-        <v>96.5</v>
+        <v>97.3</v>
       </c>
       <c r="D4">
-        <v>96.4</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="5" spans="1:6">

</xml_diff>